<commit_message>
New .xlsx with changed data types (see issue #8)
</commit_message>
<xml_diff>
--- a/inputfiles_overview.xlsx
+++ b/inputfiles_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\UAS\01__Masterthesis\05_Tests\20211029_Plugin\create_bluem_input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgrosshaus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7295D738-7EA7-4CDF-B41E-BA2D6F3A73F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5C7EAE-A017-456C-B8C1-81868026B5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="6870" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputfiles_overview" sheetId="3" r:id="rId1"/>
@@ -3414,10 +3414,10 @@
   <dimension ref="A1:FS25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FB21" sqref="FB21"/>
+      <selection pane="bottomRight" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7040,7 +7040,7 @@
         <v>312</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>503</v>
+        <v>396</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>313</v>
@@ -7052,7 +7052,7 @@
         <v>314</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="X21" s="1" t="s">
         <v>315</v>
@@ -7064,7 +7064,7 @@
         <v>316</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="AB21" s="1" t="s">
         <v>317</v>
@@ -7076,7 +7076,7 @@
         <v>318</v>
       </c>
       <c r="AE21" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="AF21" s="1" t="s">
         <v>319</v>
@@ -7088,7 +7088,7 @@
         <v>320</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="AJ21" s="1" t="s">
         <v>321</v>
@@ -7100,7 +7100,7 @@
         <v>322</v>
       </c>
       <c r="AM21" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="AN21" s="1" t="s">
         <v>323</v>
@@ -7112,7 +7112,7 @@
         <v>324</v>
       </c>
       <c r="AQ21" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="AR21" s="1" t="s">
         <v>84</v>
@@ -7167,7 +7167,7 @@
         <v>326</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="V22" s="1" t="s">
         <v>327</v>

</xml_diff>